<commit_message>
Hoàn thiện Ngoại Trú
</commit_message>
<xml_diff>
--- a/DataTest/Tiếp nhận/TC_01.xlsx
+++ b/DataTest/Tiếp nhận/TC_01.xlsx
@@ -5,34 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanh Truc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HIS api automation\DataTest\Tiếp nhận\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14AC3B4B-F42E-458E-BD2F-23422E25C056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157400B5-0024-4DF6-B049-F7248DD58B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{794CA7EE-973C-4E52-B2EA-D86EA806D076}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Check" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -240,7 +224,7 @@
     <t>5/49 Ntl, Phường 07, Quận Bình Thạnh, Thành phố Hồ Chí Minh</t>
   </si>
   <si>
-    <t>DN4127460129104</t>
+    <t>DN4127460130000</t>
   </si>
   <si>
     <t>BHXH</t>
@@ -268,7 +252,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +266,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -291,7 +280,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -314,13 +303,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -636,24 +643,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64A327E-43DD-469F-A788-E92153460493}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="52.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="61.21875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="61.33203125" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="231.33203125" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="22" bestFit="1" customWidth="1"/>
@@ -843,7 +851,7 @@
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1913</v>
+        <v>3000</v>
       </c>
       <c r="B2" t="s">
         <v>60</v>
@@ -855,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>46200602605</v>
+        <v>46200608000</v>
       </c>
       <c r="F2">
         <v>356572156</v>
@@ -990,38 +998,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC7F63F-8A09-4317-BC6C-1379C0A58D70}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1913</v>
+        <v>3000</v>
       </c>
       <c r="B2" t="s">
         <v>60</v>
@@ -1040,6 +1046,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>